<commit_message>
updates on exports and calcs
</commit_message>
<xml_diff>
--- a/support/gcam_data/Electricity_mixes.xlsx
+++ b/support/gcam_data/Electricity_mixes.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/ExioSteel/support/gcam_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C6714B-6E15-3A49-A705-C50621E08C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9240" yWindow="-28300" windowWidth="51200" windowHeight="26880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -109,8 +103,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,11 +156,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -176,21 +167,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -228,7 +211,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -262,7 +245,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -297,10 +279,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -473,22 +454,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -529,124 +502,124 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D2">
-        <v>6.111196806157358E-3</v>
+        <v>0.006111196806157358</v>
       </c>
       <c r="E2">
-        <v>2.0356177127053721E-2</v>
+        <v>0.02035617712705372</v>
       </c>
       <c r="F2">
-        <v>2.9736883095852599E-2</v>
+        <v>0.0297368830958526</v>
       </c>
       <c r="G2">
-        <v>1.269299261614506E-2</v>
+        <v>0.01269299261614506</v>
       </c>
       <c r="H2">
-        <v>1.502136884124145E-2</v>
+        <v>0.01502136884124145</v>
       </c>
       <c r="I2">
-        <v>2.788572432504164E-2</v>
+        <v>0.02788572432504164</v>
       </c>
       <c r="J2">
-        <v>2.7590666736669951E-2</v>
+        <v>0.02759066673666995</v>
       </c>
       <c r="K2">
-        <v>3.20748123279469E-2</v>
+        <v>0.0320748123279469</v>
       </c>
       <c r="L2">
-        <v>3.5453634240903129E-2</v>
+        <v>0.03545363424090313</v>
       </c>
       <c r="M2">
-        <v>4.1700693893688259E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+        <v>0.04170069389368826</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D3">
-        <v>0.55969639602640198</v>
+        <v>0.559696396026402</v>
       </c>
       <c r="E3">
-        <v>0.54665379976492701</v>
+        <v>0.546653799764927</v>
       </c>
       <c r="F3">
-        <v>0.51849608410944836</v>
+        <v>0.5184960841094484</v>
       </c>
       <c r="G3">
-        <v>0.49239042555107598</v>
+        <v>0.492390425551076</v>
       </c>
       <c r="H3">
-        <v>0.31533182174999352</v>
+        <v>0.3153318217499935</v>
       </c>
       <c r="I3">
-        <v>2.313982002018514E-2</v>
+        <v>0.02313982002018514</v>
       </c>
       <c r="J3">
-        <v>2.6607597770653451E-2</v>
+        <v>0.02660759777065345</v>
       </c>
       <c r="K3">
-        <v>2.9673013433055281E-2</v>
+        <v>0.02967301343305528</v>
       </c>
       <c r="L3">
-        <v>2.873113043328069E-2</v>
+        <v>0.02873113043328069</v>
       </c>
       <c r="M3">
-        <v>1.4875269443025771E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+        <v>0.01487526944302577</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D4">
-        <v>8.2638752524127501E-2</v>
+        <v>0.0826387525241275</v>
       </c>
       <c r="E4">
-        <v>8.0133341235596539E-2</v>
+        <v>0.08013334123559654</v>
       </c>
       <c r="F4">
-        <v>6.9860168091991526E-2</v>
+        <v>0.06986016809199153</v>
       </c>
       <c r="G4">
-        <v>3.4711616893438553E-2</v>
+        <v>0.03471161689343855</v>
       </c>
       <c r="H4">
-        <v>2.3577554334068249E-2</v>
+        <v>0.02357755433406825</v>
       </c>
       <c r="I4">
-        <v>1.517282030910286E-2</v>
+        <v>0.01517282030910286</v>
       </c>
       <c r="J4">
-        <v>1.8206352207473561E-2</v>
+        <v>0.01820635220747356</v>
       </c>
       <c r="K4">
-        <v>1.9123594319466169E-2</v>
+        <v>0.01912359431946617</v>
       </c>
       <c r="L4">
-        <v>1.6586320823334371E-2</v>
+        <v>0.01658632082333437</v>
       </c>
       <c r="M4">
-        <v>9.0521112120035777E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+        <v>0.009052111212003578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
@@ -657,33 +630,33 @@
         <v>0.1182063477155845</v>
       </c>
       <c r="F5">
-        <v>9.5267378760850896E-2</v>
+        <v>0.0952673787608509</v>
       </c>
       <c r="G5">
-        <v>8.9617496288355497E-2</v>
+        <v>0.0896174962883555</v>
       </c>
       <c r="H5">
-        <v>8.0093840905438432E-2</v>
+        <v>0.08009384090543843</v>
       </c>
       <c r="I5">
-        <v>7.7861499259783334E-2</v>
+        <v>0.07786149925978333</v>
       </c>
       <c r="J5">
-        <v>6.6914135299566677E-2</v>
+        <v>0.06691413529956668</v>
       </c>
       <c r="K5">
-        <v>5.8733236333094338E-2</v>
+        <v>0.05873323633309434</v>
       </c>
       <c r="L5">
-        <v>5.4156322321287018E-2</v>
+        <v>0.05415632232128702</v>
       </c>
       <c r="M5">
-        <v>5.1188205966468878E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+        <v>0.05118820596646888</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
@@ -691,297 +664,297 @@
         <v>0.2162691048593598</v>
       </c>
       <c r="E6">
-        <v>0.19954699045935931</v>
+        <v>0.1995469904593593</v>
       </c>
       <c r="F6">
-        <v>0.20290676391408169</v>
+        <v>0.2029067639140817</v>
       </c>
       <c r="G6">
-        <v>0.18249700849866249</v>
+        <v>0.1824970084986625</v>
       </c>
       <c r="H6">
         <v>0.169289537802536</v>
       </c>
       <c r="I6">
-        <v>0.18430077586532889</v>
+        <v>0.1843007758653289</v>
       </c>
       <c r="J6">
         <v>0.1757070443241413</v>
       </c>
       <c r="K6">
-        <v>0.15832704366925859</v>
+        <v>0.1583270436692586</v>
       </c>
       <c r="L6">
         <v>0.1440736958251857</v>
       </c>
       <c r="M6">
-        <v>0.13180295094271649</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+        <v>0.1318029509427165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D7">
-        <v>2.6718865368589681E-2</v>
+        <v>0.02671886536858968</v>
       </c>
       <c r="E7">
-        <v>2.4307024033200241E-2</v>
+        <v>0.02430702403320024</v>
       </c>
       <c r="F7">
-        <v>1.5796700428466971E-2</v>
+        <v>0.01579670042846697</v>
       </c>
       <c r="G7">
-        <v>8.4348228141609485E-3</v>
+        <v>0.008434822814160949</v>
       </c>
       <c r="H7">
-        <v>7.7734230023658443E-3</v>
+        <v>0.007773423002365844</v>
       </c>
       <c r="I7">
-        <v>1.033505616963294E-2</v>
+        <v>0.01033505616963294</v>
       </c>
       <c r="J7">
-        <v>9.8393352222390183E-3</v>
+        <v>0.009839335222239018</v>
       </c>
       <c r="K7">
-        <v>6.3651649702039974E-3</v>
+        <v>0.006365164970203997</v>
       </c>
       <c r="L7">
-        <v>4.1743620923567794E-3</v>
+        <v>0.004174362092356779</v>
       </c>
       <c r="M7">
-        <v>2.7958980589846091E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+        <v>0.002795898058984609</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="G8">
-        <v>5.3927056164761612E-3</v>
+        <v>0.005392705616476161</v>
       </c>
       <c r="H8">
-        <v>1.1327819003792219E-2</v>
+        <v>0.01132781900379222</v>
       </c>
       <c r="I8">
-        <v>1.8012697564739489E-2</v>
+        <v>0.01801269756473949</v>
       </c>
       <c r="J8">
-        <v>1.993347315210011E-2</v>
+        <v>0.01993347315210011</v>
       </c>
       <c r="K8">
-        <v>1.806350973076732E-2</v>
+        <v>0.01806350973076732</v>
       </c>
       <c r="L8">
-        <v>1.580768220756636E-2</v>
+        <v>0.01580768220756636</v>
       </c>
       <c r="M8">
-        <v>1.296203760396103E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+        <v>0.01296203760396103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D9">
-        <v>2.2360774608925441E-6</v>
+        <v>2.236077460892544E-06</v>
       </c>
       <c r="E9">
-        <v>1.471425403057365E-3</v>
+        <v>0.001471425403057365</v>
       </c>
       <c r="F9">
-        <v>1.560166789281401E-2</v>
+        <v>0.01560166789281401</v>
       </c>
       <c r="G9">
-        <v>2.6981346757533171E-2</v>
+        <v>0.02698134675753317</v>
       </c>
       <c r="H9">
-        <v>0.14485733829161859</v>
+        <v>0.1448573382916186</v>
       </c>
       <c r="I9">
-        <v>0.32216012583037562</v>
+        <v>0.3221601258303756</v>
       </c>
       <c r="J9">
-        <v>0.29472510875867469</v>
+        <v>0.2947251087586747</v>
       </c>
       <c r="K9">
-        <v>0.29095808914241827</v>
+        <v>0.2909580891424183</v>
       </c>
       <c r="L9">
-        <v>0.29481872229708078</v>
+        <v>0.2948187222970808</v>
       </c>
       <c r="M9">
-        <v>0.31468428737355159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+        <v>0.3146842873735516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D10">
-        <v>6.4846507240138261E-4</v>
+        <v>0.0006484650724013826</v>
       </c>
       <c r="E10">
-        <v>9.3248942612213087E-3</v>
+        <v>0.009324894261221309</v>
       </c>
       <c r="F10">
-        <v>5.2334353706493912E-2</v>
+        <v>0.05233435370649391</v>
       </c>
       <c r="G10">
-        <v>0.14728158496415211</v>
+        <v>0.1472815849641521</v>
       </c>
       <c r="H10">
-        <v>0.23272729606894571</v>
+        <v>0.2327272960689457</v>
       </c>
       <c r="I10">
         <v>0.3211314806558101</v>
       </c>
       <c r="J10">
-        <v>0.36047628652848118</v>
+        <v>0.3604762865284812</v>
       </c>
       <c r="K10">
-        <v>0.38668153607378902</v>
+        <v>0.386681536073789</v>
       </c>
       <c r="L10">
-        <v>0.40619812975900499</v>
+        <v>0.406198129759005</v>
       </c>
       <c r="M10">
-        <v>0.42093854550559978</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+        <v>0.4209385455055998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D11">
-        <v>1.785906178492112E-2</v>
+        <v>0.01785906178492112</v>
       </c>
       <c r="E11">
-        <v>2.8010555326487122E-2</v>
+        <v>0.02801055532648712</v>
       </c>
       <c r="F11">
-        <v>3.016754530783124E-2</v>
+        <v>0.03016754530783124</v>
       </c>
       <c r="G11">
-        <v>1.101068180667408E-2</v>
+        <v>0.01101068180667408</v>
       </c>
       <c r="H11">
-        <v>1.096514060516591E-2</v>
+        <v>0.01096514060516591</v>
       </c>
       <c r="I11">
-        <v>9.9766213768876857E-3</v>
+        <v>0.009976621376887686</v>
       </c>
       <c r="J11">
-        <v>1.4340718990696159E-2</v>
+        <v>0.01434071899069616</v>
       </c>
       <c r="K11">
-        <v>1.9537863415983049E-2</v>
+        <v>0.01953786341598305</v>
       </c>
       <c r="L11">
-        <v>2.3046677555952699E-2</v>
+        <v>0.0230466775559527</v>
       </c>
       <c r="M11">
-        <v>2.4339196803294438E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+        <v>0.02433919680329444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D12">
-        <v>0.25688365386153028</v>
+        <v>0.2568836538615303</v>
       </c>
       <c r="E12">
-        <v>0.20889703067180029</v>
+        <v>0.2088970306718003</v>
       </c>
       <c r="F12">
-        <v>0.22132362516024581</v>
+        <v>0.2213236251602458</v>
       </c>
       <c r="G12">
-        <v>0.16476936813768989</v>
+        <v>0.1647693681376899</v>
       </c>
       <c r="H12">
-        <v>9.2084769878816766E-2</v>
+        <v>0.09208476987881677</v>
       </c>
       <c r="I12">
-        <v>1.515882668046838E-3</v>
+        <v>0.001515882668046838</v>
       </c>
       <c r="J12">
-        <v>1.9600596584597582E-3</v>
+        <v>0.001960059658459758</v>
       </c>
       <c r="K12">
-        <v>2.0883960351821278E-3</v>
+        <v>0.002088396035182128</v>
       </c>
       <c r="L12">
-        <v>1.0416021349776261E-3</v>
+        <v>0.001041602134977626</v>
       </c>
       <c r="M12">
-        <v>1.9634196328052709E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+        <v>0.0001963419632805271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D13">
-        <v>0.17687033328297669</v>
+        <v>0.1768703332829767</v>
       </c>
       <c r="E13">
         <v>0.2050483213169334</v>
       </c>
       <c r="F13">
-        <v>0.13971771430441729</v>
+        <v>0.1397177143044173</v>
       </c>
       <c r="G13">
-        <v>8.7708165104314881E-2</v>
+        <v>0.08770816510431488</v>
       </c>
       <c r="H13">
-        <v>2.9563834222922358E-2</v>
+        <v>0.02956383422292236</v>
       </c>
       <c r="I13">
-        <v>3.752036366644864E-3</v>
+        <v>0.003752036366644864</v>
       </c>
       <c r="J13">
-        <v>2.8523414801268189E-3</v>
+        <v>0.002852341480126819</v>
       </c>
       <c r="K13">
-        <v>2.2156868829701212E-3</v>
+        <v>0.002215686882970121</v>
       </c>
       <c r="L13">
-        <v>1.3593924870245969E-3</v>
+        <v>0.001359392487024597</v>
       </c>
       <c r="M13">
-        <v>5.2528198001748714E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+        <v>0.0005252819800174871</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>22</v>
       </c>
@@ -989,10 +962,10 @@
         <v>0.1142238515239314</v>
       </c>
       <c r="E14">
-        <v>0.13748800473848591</v>
+        <v>0.1374880047384859</v>
       </c>
       <c r="F14">
-        <v>0.13045964957625031</v>
+        <v>0.1304596495762503</v>
       </c>
       <c r="G14">
         <v>0.1307371385261705</v>
@@ -1001,324 +974,324 @@
         <v>0.1132273401965741</v>
       </c>
       <c r="I14">
-        <v>0.10070648758449351</v>
+        <v>0.1007064875844935</v>
       </c>
       <c r="J14">
-        <v>8.4719962722760667E-2</v>
+        <v>0.08471996272276067</v>
       </c>
       <c r="K14">
-        <v>7.1259536034611728E-2</v>
+        <v>0.07125953603461173</v>
       </c>
       <c r="L14">
-        <v>6.2423814629754187E-2</v>
+        <v>0.06242381462975419</v>
       </c>
       <c r="M14">
-        <v>5.6024601624713379E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+        <v>0.05602460162471338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D15">
-        <v>0.35909388046385382</v>
+        <v>0.3590938804638538</v>
       </c>
       <c r="E15">
-        <v>0.32805807533420822</v>
+        <v>0.3280580753342082</v>
       </c>
       <c r="F15">
-        <v>0.30887264850045698</v>
+        <v>0.308872648500457</v>
       </c>
       <c r="G15">
-        <v>0.29207893954587938</v>
+        <v>0.2920789395458794</v>
       </c>
       <c r="H15">
-        <v>0.26398153966667798</v>
+        <v>0.263981539666678</v>
       </c>
       <c r="I15">
-        <v>0.23965235711200769</v>
+        <v>0.2396523571120077</v>
       </c>
       <c r="J15">
         <v>0.2087558309049321</v>
       </c>
       <c r="K15">
-        <v>0.17568977178699011</v>
+        <v>0.1756897717869901</v>
       </c>
       <c r="L15">
-        <v>0.14891846743527479</v>
+        <v>0.1489184674352748</v>
       </c>
       <c r="M15">
         <v>0.1233744798737219</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D16">
-        <v>4.2588426355205149E-2</v>
+        <v>0.04258842635520515</v>
       </c>
       <c r="E16">
-        <v>2.247105381612529E-2</v>
+        <v>0.02247105381612529</v>
       </c>
       <c r="F16">
-        <v>1.9125103942189799E-2</v>
+        <v>0.0191251039421898</v>
       </c>
       <c r="G16">
-        <v>4.5556370259311994E-3</v>
+        <v>0.004555637025931199</v>
       </c>
       <c r="H16">
-        <v>2.096727292098235E-3</v>
+        <v>0.002096727292098235</v>
       </c>
       <c r="I16">
-        <v>1.435302719269856E-3</v>
+        <v>0.001435302719269856</v>
       </c>
       <c r="J16">
-        <v>1.86127625495947E-3</v>
+        <v>0.00186127625495947</v>
       </c>
       <c r="K16">
-        <v>1.359651715918578E-3</v>
+        <v>0.001359651715918578</v>
       </c>
       <c r="L16">
-        <v>8.7947865756692978E-4</v>
+        <v>0.0008794786575669298</v>
       </c>
       <c r="M16">
-        <v>3.7207874554899702E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+        <v>0.000372078745548997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D17">
-        <v>2.3652877936551171E-3</v>
+        <v>0.002365287793655117</v>
       </c>
       <c r="E17">
-        <v>2.406708427390982E-3</v>
+        <v>0.002406708427390982</v>
       </c>
       <c r="F17">
-        <v>2.934854985206594E-3</v>
+        <v>0.002934854985206594</v>
       </c>
       <c r="G17">
-        <v>1.1665697411576151E-2</v>
+        <v>0.01166569741157615</v>
       </c>
       <c r="H17">
-        <v>1.538310548301697E-2</v>
+        <v>0.01538310548301697</v>
       </c>
       <c r="I17">
-        <v>1.605487133534517E-2</v>
+        <v>0.01605487133534517</v>
       </c>
       <c r="J17">
-        <v>1.732479417010082E-2</v>
+        <v>0.01732479417010082</v>
       </c>
       <c r="K17">
-        <v>1.473849926289662E-2</v>
+        <v>0.01473849926289662</v>
       </c>
       <c r="L17">
-        <v>1.151660184922333E-2</v>
+        <v>0.01151660184922333</v>
       </c>
       <c r="M17">
-        <v>7.9030428122916808E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+        <v>0.007903042812291681</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D18">
-        <v>6.3898284017362649E-4</v>
+        <v>0.0006389828401736265</v>
       </c>
       <c r="E18">
-        <v>9.6904195248109504E-3</v>
+        <v>0.00969041952481095</v>
       </c>
       <c r="F18">
-        <v>4.1654964749589581E-2</v>
+        <v>0.04165496474958958</v>
       </c>
       <c r="G18">
-        <v>5.3235554429344772E-2</v>
+        <v>0.05323555442934477</v>
       </c>
       <c r="H18">
         <v>0.1491852344740297</v>
       </c>
       <c r="I18">
-        <v>0.23526641065005571</v>
+        <v>0.2352664106500557</v>
       </c>
       <c r="J18">
         <v>0.2374049217090401</v>
       </c>
       <c r="K18">
-        <v>0.25007014666173127</v>
+        <v>0.2500701466617313</v>
       </c>
       <c r="L18">
-        <v>0.28141918840177221</v>
+        <v>0.2814191884017722</v>
       </c>
       <c r="M18">
-        <v>0.34533993382244371</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+        <v>0.3453399338224437</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D19">
-        <v>2.9476522093752872E-2</v>
+        <v>0.02947652209375287</v>
       </c>
       <c r="E19">
-        <v>5.7929830843757753E-2</v>
+        <v>0.05792983084375775</v>
       </c>
       <c r="F19">
         <v>0.1057438934738123</v>
       </c>
       <c r="G19">
-        <v>0.24423881801241909</v>
+        <v>0.2442388180124191</v>
       </c>
       <c r="H19">
-        <v>0.32351230818069793</v>
+        <v>0.3235123081806979</v>
       </c>
       <c r="I19">
-        <v>0.39164003018724852</v>
+        <v>0.3916400301872485</v>
       </c>
       <c r="J19">
-        <v>0.43078009410892409</v>
+        <v>0.4307800941089241</v>
       </c>
       <c r="K19">
-        <v>0.46304044820371631</v>
+        <v>0.4630404482037163</v>
       </c>
       <c r="L19">
-        <v>0.46939477684845371</v>
+        <v>0.4693947768484537</v>
       </c>
       <c r="M19">
-        <v>0.44192504237468783</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+        <v>0.4419250423746878</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D20">
-        <v>6.111196806157358E-3</v>
+        <v>0.006111196806157358</v>
       </c>
       <c r="E20">
-        <v>2.0356177127053721E-2</v>
+        <v>0.02035617712705372</v>
       </c>
       <c r="F20">
-        <v>2.9736883095852599E-2</v>
+        <v>0.0297368830958526</v>
       </c>
       <c r="G20">
-        <v>1.269299261614506E-2</v>
+        <v>0.01269299261614506</v>
       </c>
       <c r="H20">
-        <v>1.502136884124145E-2</v>
+        <v>0.01502136884124145</v>
       </c>
       <c r="I20">
-        <v>2.8732707263530621E-2</v>
+        <v>0.02873270726353062</v>
       </c>
       <c r="J20">
-        <v>2.7631438665879849E-2</v>
+        <v>0.02763143866587985</v>
       </c>
       <c r="K20">
-        <v>3.2075873500494623E-2</v>
+        <v>0.03207587350049462</v>
       </c>
       <c r="L20">
-        <v>3.5409680558125489E-2</v>
+        <v>0.03540968055812549</v>
       </c>
       <c r="M20">
-        <v>4.1660951748039403E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+        <v>0.0416609517480394</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D21">
-        <v>0.55969639602640198</v>
+        <v>0.559696396026402</v>
       </c>
       <c r="E21">
-        <v>0.54665379976492701</v>
+        <v>0.546653799764927</v>
       </c>
       <c r="F21">
-        <v>0.51849608410944836</v>
+        <v>0.5184960841094484</v>
       </c>
       <c r="G21">
-        <v>0.49239042555107598</v>
+        <v>0.492390425551076</v>
       </c>
       <c r="H21">
-        <v>0.31533182174999352</v>
+        <v>0.3153318217499935</v>
       </c>
       <c r="I21">
-        <v>2.1338908975428821E-2</v>
+        <v>0.02133890897542882</v>
       </c>
       <c r="J21">
-        <v>2.6980428828190971E-2</v>
+        <v>0.02698042882819097</v>
       </c>
       <c r="K21">
-        <v>2.9961628701594151E-2</v>
+        <v>0.02996162870159415</v>
       </c>
       <c r="L21">
-        <v>2.8906194373283491E-2</v>
+        <v>0.02890619437328349</v>
       </c>
       <c r="M21">
-        <v>1.4855196989389349E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+        <v>0.01485519698938935</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D22">
-        <v>8.2638752524127501E-2</v>
+        <v>0.0826387525241275</v>
       </c>
       <c r="E22">
-        <v>8.0133341235596539E-2</v>
+        <v>0.08013334123559654</v>
       </c>
       <c r="F22">
-        <v>6.9860168091991526E-2</v>
+        <v>0.06986016809199153</v>
       </c>
       <c r="G22">
-        <v>3.4711616893438553E-2</v>
+        <v>0.03471161689343855</v>
       </c>
       <c r="H22">
-        <v>2.3577554334068249E-2</v>
+        <v>0.02357755433406825</v>
       </c>
       <c r="I22">
-        <v>1.507725032579905E-2</v>
+        <v>0.01507725032579905</v>
       </c>
       <c r="J22">
-        <v>1.8814669921232562E-2</v>
+        <v>0.01881466992123256</v>
       </c>
       <c r="K22">
-        <v>1.9583136864912941E-2</v>
+        <v>0.01958313686491294</v>
       </c>
       <c r="L22">
-        <v>1.6875435586498951E-2</v>
+        <v>0.01687543558649895</v>
       </c>
       <c r="M22">
-        <v>9.1536527934586408E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+        <v>0.009153652793458641</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1329,33 +1302,33 @@
         <v>0.1182063477155845</v>
       </c>
       <c r="F23">
-        <v>9.5267378760850896E-2</v>
+        <v>0.0952673787608509</v>
       </c>
       <c r="G23">
-        <v>8.9617496288355497E-2</v>
+        <v>0.0896174962883555</v>
       </c>
       <c r="H23">
-        <v>8.0093840905438432E-2</v>
+        <v>0.08009384090543843</v>
       </c>
       <c r="I23">
-        <v>7.794299305750621E-2</v>
+        <v>0.07794299305750621</v>
       </c>
       <c r="J23">
-        <v>6.6795858454679335E-2</v>
+        <v>0.06679585845467934</v>
       </c>
       <c r="K23">
-        <v>5.8637214128331783E-2</v>
+        <v>0.05863721412833178</v>
       </c>
       <c r="L23">
-        <v>5.4094758440244972E-2</v>
+        <v>0.05409475844024497</v>
       </c>
       <c r="M23">
-        <v>5.1154407893760342E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+        <v>0.05115440789376034</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1363,19 +1336,19 @@
         <v>0.2162691048593598</v>
       </c>
       <c r="E24">
-        <v>0.19954699045935931</v>
+        <v>0.1995469904593593</v>
       </c>
       <c r="F24">
-        <v>0.20290676391408169</v>
+        <v>0.2029067639140817</v>
       </c>
       <c r="G24">
-        <v>0.18249700849866249</v>
+        <v>0.1824970084986625</v>
       </c>
       <c r="H24">
         <v>0.169289537802536</v>
       </c>
       <c r="I24">
-        <v>0.18553788119723649</v>
+        <v>0.1855378811972365</v>
       </c>
       <c r="J24">
         <v>0.1763131319405542</v>
@@ -1384,276 +1357,276 @@
         <v>0.1588448775131118</v>
       </c>
       <c r="L24">
-        <v>0.14458643513991981</v>
+        <v>0.1445864351399198</v>
       </c>
       <c r="M24">
-        <v>0.13233287531456481</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+        <v>0.1323328753145648</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D25">
-        <v>2.6718865368589681E-2</v>
+        <v>0.02671886536858968</v>
       </c>
       <c r="E25">
-        <v>2.4307024033200241E-2</v>
+        <v>0.02430702403320024</v>
       </c>
       <c r="F25">
-        <v>1.5796700428466971E-2</v>
+        <v>0.01579670042846697</v>
       </c>
       <c r="G25">
-        <v>8.4348228141609485E-3</v>
+        <v>0.008434822814160949</v>
       </c>
       <c r="H25">
-        <v>7.7734230023658443E-3</v>
+        <v>0.007773423002365844</v>
       </c>
       <c r="I25">
-        <v>1.0565883037876721E-2</v>
+        <v>0.01056588303787672</v>
       </c>
       <c r="J25">
-        <v>9.8410673783073336E-3</v>
+        <v>0.009841067378307334</v>
       </c>
       <c r="K25">
-        <v>6.3559715475577407E-3</v>
+        <v>0.006355971547557741</v>
       </c>
       <c r="L25">
-        <v>4.1633234941985059E-3</v>
+        <v>0.004163323494198506</v>
       </c>
       <c r="M25">
-        <v>2.795594230610174E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+        <v>0.002795594230610174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="G26">
-        <v>5.3927056164761612E-3</v>
+        <v>0.005392705616476161</v>
       </c>
       <c r="H26">
-        <v>1.1327819003792219E-2</v>
+        <v>0.01132781900379222</v>
       </c>
       <c r="I26">
-        <v>1.8188740583216859E-2</v>
+        <v>0.01818874058321686</v>
       </c>
       <c r="J26">
-        <v>1.995239215025579E-2</v>
+        <v>0.01995239215025579</v>
       </c>
       <c r="K26">
-        <v>1.8054716364485419E-2</v>
+        <v>0.01805471636448542</v>
       </c>
       <c r="L26">
-        <v>1.5799688786656309E-2</v>
+        <v>0.01579968878665631</v>
       </c>
       <c r="M26">
-        <v>1.296132023936163E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+        <v>0.01296132023936163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D27">
-        <v>2.2360774608925441E-6</v>
+        <v>2.236077460892544E-06</v>
       </c>
       <c r="E27">
-        <v>1.471425403057365E-3</v>
+        <v>0.001471425403057365</v>
       </c>
       <c r="F27">
-        <v>1.560166789281401E-2</v>
+        <v>0.01560166789281401</v>
       </c>
       <c r="G27">
-        <v>2.6981346757533171E-2</v>
+        <v>0.02698134675753317</v>
       </c>
       <c r="H27">
-        <v>0.14485733829161859</v>
+        <v>0.1448573382916186</v>
       </c>
       <c r="I27">
-        <v>0.32138049579271588</v>
+        <v>0.3213804957927159</v>
       </c>
       <c r="J27">
-        <v>0.29358782479705392</v>
+        <v>0.2935878247970539</v>
       </c>
       <c r="K27">
-        <v>0.29013494852277583</v>
+        <v>0.2901349485227758</v>
       </c>
       <c r="L27">
-        <v>0.29422678683111619</v>
+        <v>0.2942267868311162</v>
       </c>
       <c r="M27">
-        <v>0.31426637340490732</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+        <v>0.3142663734049073</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D28">
-        <v>6.4846507240138261E-4</v>
+        <v>0.0006484650724013826</v>
       </c>
       <c r="E28">
-        <v>9.3248942612213087E-3</v>
+        <v>0.009324894261221309</v>
       </c>
       <c r="F28">
-        <v>5.2334353706493912E-2</v>
+        <v>0.05233435370649391</v>
       </c>
       <c r="G28">
-        <v>0.14728158496415211</v>
+        <v>0.1472815849641521</v>
       </c>
       <c r="H28">
-        <v>0.23272729606894571</v>
+        <v>0.2327272960689457</v>
       </c>
       <c r="I28">
-        <v>0.32123513976668938</v>
+        <v>0.3212351397666894</v>
       </c>
       <c r="J28">
-        <v>0.36008318786384608</v>
+        <v>0.3600831878638461</v>
       </c>
       <c r="K28">
-        <v>0.38635163285673579</v>
+        <v>0.3863516328567358</v>
       </c>
       <c r="L28">
-        <v>0.40593769678995628</v>
+        <v>0.4059376967899563</v>
       </c>
       <c r="M28">
         <v>0.4208196273859085</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2" t="s">
+    <row r="29" spans="1:13">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D29">
-        <v>1.785906178492112E-2</v>
+        <v>0.01785906178492112</v>
       </c>
       <c r="E29">
-        <v>2.8010555326487122E-2</v>
+        <v>0.02801055532648712</v>
       </c>
       <c r="F29">
-        <v>3.016754530783124E-2</v>
+        <v>0.03016754530783124</v>
       </c>
       <c r="G29">
-        <v>1.101068180667408E-2</v>
+        <v>0.01101068180667408</v>
       </c>
       <c r="H29">
-        <v>1.096514060516591E-2</v>
+        <v>0.01096514060516591</v>
       </c>
       <c r="I29">
-        <v>1.0380141601467481E-2</v>
+        <v>0.01038014160146748</v>
       </c>
       <c r="J29">
-        <v>1.4360894175291969E-2</v>
+        <v>0.01436089417529197</v>
       </c>
       <c r="K29">
-        <v>1.9540090599796792E-2</v>
+        <v>0.01954009059979679</v>
       </c>
       <c r="L29">
-        <v>2.3024768875265261E-2</v>
+        <v>0.02302476887526526</v>
       </c>
       <c r="M29">
-        <v>2.4317219767583761E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+        <v>0.02431721976758376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D30">
-        <v>0.25688365386153028</v>
+        <v>0.2568836538615303</v>
       </c>
       <c r="E30">
-        <v>0.20889703067180029</v>
+        <v>0.2088970306718003</v>
       </c>
       <c r="F30">
-        <v>0.22132362516024581</v>
+        <v>0.2213236251602458</v>
       </c>
       <c r="G30">
-        <v>0.16476936813768989</v>
+        <v>0.1647693681376899</v>
       </c>
       <c r="H30">
-        <v>9.2084769878816766E-2</v>
+        <v>0.09208476987881677</v>
       </c>
       <c r="I30">
-        <v>1.430375010920137E-3</v>
+        <v>0.001430375010920137</v>
       </c>
       <c r="J30">
-        <v>1.9805626279198961E-3</v>
+        <v>0.001980562627919896</v>
       </c>
       <c r="K30">
-        <v>2.100687048299266E-3</v>
+        <v>0.002100687048299266</v>
       </c>
       <c r="L30">
-        <v>1.03843597026182E-3</v>
+        <v>0.00103843597026182</v>
       </c>
       <c r="M30">
-        <v>1.9536022010891371E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+        <v>0.0001953602201089137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D31">
-        <v>0.17687033328297669</v>
+        <v>0.1768703332829767</v>
       </c>
       <c r="E31">
         <v>0.2050483213169334</v>
       </c>
       <c r="F31">
-        <v>0.13971771430441729</v>
+        <v>0.1397177143044173</v>
       </c>
       <c r="G31">
-        <v>8.7708165104314881E-2</v>
+        <v>0.08770816510431488</v>
       </c>
       <c r="H31">
-        <v>2.9563834222922358E-2</v>
+        <v>0.02956383422292236</v>
       </c>
       <c r="I31">
-        <v>3.3637223011915999E-3</v>
+        <v>0.0033637223011916</v>
       </c>
       <c r="J31">
-        <v>2.9155634433511782E-3</v>
+        <v>0.002915563443351178</v>
       </c>
       <c r="K31">
-        <v>2.2512294992873489E-3</v>
+        <v>0.002251229499287349</v>
       </c>
       <c r="L31">
-        <v>1.3664265297804489E-3</v>
+        <v>0.001366426529780449</v>
       </c>
       <c r="M31">
-        <v>5.2477103347020018E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+        <v>0.0005247710334702002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
         <v>22</v>
       </c>
@@ -1661,10 +1634,10 @@
         <v>0.1142238515239314</v>
       </c>
       <c r="E32">
-        <v>0.13748800473848591</v>
+        <v>0.1374880047384859</v>
       </c>
       <c r="F32">
-        <v>0.13045964957625031</v>
+        <v>0.1304596495762503</v>
       </c>
       <c r="G32">
         <v>0.1307371385261705</v>
@@ -1676,321 +1649,321 @@
         <v>0.1006034754922057</v>
       </c>
       <c r="J32">
-        <v>8.4576924376808138E-2</v>
+        <v>0.08457692437680814</v>
       </c>
       <c r="K32">
-        <v>7.1139376891711847E-2</v>
+        <v>0.07113937689171185</v>
       </c>
       <c r="L32">
-        <v>6.2348766180040052E-2</v>
+        <v>0.06234876618004005</v>
       </c>
       <c r="M32">
-        <v>5.5978722006857787E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+        <v>0.05597872200685779</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D33">
-        <v>0.35909388046385382</v>
+        <v>0.3590938804638538</v>
       </c>
       <c r="E33">
-        <v>0.32805807533420822</v>
+        <v>0.3280580753342082</v>
       </c>
       <c r="F33">
-        <v>0.30887264850045698</v>
+        <v>0.308872648500457</v>
       </c>
       <c r="G33">
-        <v>0.29207893954587938</v>
+        <v>0.2920789395458794</v>
       </c>
       <c r="H33">
-        <v>0.26398153966667798</v>
+        <v>0.263981539666678</v>
       </c>
       <c r="I33">
-        <v>0.24002454182167679</v>
+        <v>0.2400245418216768</v>
       </c>
       <c r="J33">
-        <v>0.20899249658076111</v>
+        <v>0.2089924965807611</v>
       </c>
       <c r="K33">
-        <v>0.17591357383192319</v>
+        <v>0.1759135738319232</v>
       </c>
       <c r="L33">
-        <v>0.14918501027729081</v>
+        <v>0.1491850102772908</v>
       </c>
       <c r="M33">
         <v>0.1236666001594242</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+    <row r="34" spans="1:13">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D34">
-        <v>4.2588426355205149E-2</v>
+        <v>0.04258842635520515</v>
       </c>
       <c r="E34">
-        <v>2.247105381612529E-2</v>
+        <v>0.02247105381612529</v>
       </c>
       <c r="F34">
-        <v>1.9125103942189799E-2</v>
+        <v>0.0191251039421898</v>
       </c>
       <c r="G34">
-        <v>4.5556370259311994E-3</v>
+        <v>0.004555637025931199</v>
       </c>
       <c r="H34">
-        <v>2.096727292098235E-3</v>
+        <v>0.002096727292098235</v>
       </c>
       <c r="I34">
-        <v>1.4675531987425501E-3</v>
+        <v>0.00146755319874255</v>
       </c>
       <c r="J34">
-        <v>1.863236206023837E-3</v>
+        <v>0.001863236206023837</v>
       </c>
       <c r="K34">
-        <v>1.3588333483972759E-3</v>
+        <v>0.001358833348397276</v>
       </c>
       <c r="L34">
-        <v>8.7681016130053955E-4</v>
+        <v>0.0008768101613005396</v>
       </c>
       <c r="M34">
-        <v>3.7143236254047522E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+        <v>0.0003714323625404752</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D35">
-        <v>2.3652877936551171E-3</v>
+        <v>0.002365287793655117</v>
       </c>
       <c r="E35">
-        <v>2.406708427390982E-3</v>
+        <v>0.002406708427390982</v>
       </c>
       <c r="F35">
-        <v>2.934854985206594E-3</v>
+        <v>0.002934854985206594</v>
       </c>
       <c r="G35">
-        <v>1.1665697411576151E-2</v>
+        <v>0.01166569741157615</v>
       </c>
       <c r="H35">
-        <v>1.538310548301697E-2</v>
+        <v>0.01538310548301697</v>
       </c>
       <c r="I35">
-        <v>1.620114900241118E-2</v>
+        <v>0.01620114900241118</v>
       </c>
       <c r="J35">
-        <v>1.7320697912094968E-2</v>
+        <v>0.01732069791209497</v>
       </c>
       <c r="K35">
-        <v>1.472720021166333E-2</v>
+        <v>0.01472720021166333</v>
       </c>
       <c r="L35">
-        <v>1.150856100704451E-2</v>
+        <v>0.01150856100704451</v>
       </c>
       <c r="M35">
-        <v>7.8996593405850062E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+        <v>0.007899659340585006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D36">
-        <v>6.3898284017362649E-4</v>
+        <v>0.0006389828401736265</v>
       </c>
       <c r="E36">
-        <v>9.6904195248109504E-3</v>
+        <v>0.00969041952481095</v>
       </c>
       <c r="F36">
-        <v>4.1654964749589581E-2</v>
+        <v>0.04165496474958958</v>
       </c>
       <c r="G36">
-        <v>5.3235554429344772E-2</v>
+        <v>0.05323555442934477</v>
       </c>
       <c r="H36">
         <v>0.1491852344740297</v>
       </c>
       <c r="I36">
-        <v>0.23524466706573141</v>
+        <v>0.2352446670657314</v>
       </c>
       <c r="J36">
-        <v>0.23740107230096749</v>
+        <v>0.2374010723009675</v>
       </c>
       <c r="K36">
-        <v>0.25007128268593992</v>
+        <v>0.2500712826859399</v>
       </c>
       <c r="L36">
-        <v>0.28137286363763148</v>
+        <v>0.2813728636376315</v>
       </c>
       <c r="M36">
-        <v>0.34520231688203162</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+        <v>0.3452023168820316</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D37">
-        <v>2.9476522093752872E-2</v>
+        <v>0.02947652209375287</v>
       </c>
       <c r="E37">
-        <v>5.7929830843757753E-2</v>
+        <v>0.05792983084375775</v>
       </c>
       <c r="F37">
         <v>0.1057438934738123</v>
       </c>
       <c r="G37">
-        <v>0.24423881801241909</v>
+        <v>0.2442388180124191</v>
       </c>
       <c r="H37">
-        <v>0.32351230818069793</v>
+        <v>0.3235123081806979</v>
       </c>
       <c r="I37">
-        <v>0.39128437450565318</v>
+        <v>0.3912843745056532</v>
       </c>
       <c r="J37">
-        <v>0.43058855237678129</v>
+        <v>0.4305885523767813</v>
       </c>
       <c r="K37">
-        <v>0.46289772588298111</v>
+        <v>0.4628977258829811</v>
       </c>
       <c r="L37">
-        <v>0.46927835736138512</v>
+        <v>0.4692783573613851</v>
       </c>
       <c r="M37">
         <v>0.4418439182273981</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:13">
+      <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D38">
-        <v>6.111196806157358E-3</v>
+        <v>0.006111196806157358</v>
       </c>
       <c r="E38">
-        <v>2.0356177127053721E-2</v>
+        <v>0.02035617712705372</v>
       </c>
       <c r="F38">
-        <v>2.9736883095852599E-2</v>
+        <v>0.0297368830958526</v>
       </c>
       <c r="G38">
-        <v>1.269299261614506E-2</v>
+        <v>0.01269299261614506</v>
       </c>
       <c r="H38">
-        <v>1.502136884124145E-2</v>
+        <v>0.01502136884124145</v>
       </c>
       <c r="I38">
-        <v>2.8866450734010091E-2</v>
+        <v>0.02886645073401009</v>
       </c>
       <c r="J38">
-        <v>2.7803572847873631E-2</v>
+        <v>0.02780357284787363</v>
       </c>
       <c r="K38">
-        <v>3.2116889961881487E-2</v>
+        <v>0.03211688996188149</v>
       </c>
       <c r="L38">
-        <v>3.531428200407595E-2</v>
+        <v>0.03531428200407595</v>
       </c>
       <c r="M38">
-        <v>4.1579077838341402E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+        <v>0.0415790778383414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D39">
-        <v>0.55969639602640198</v>
+        <v>0.559696396026402</v>
       </c>
       <c r="E39">
-        <v>0.54665379976492701</v>
+        <v>0.546653799764927</v>
       </c>
       <c r="F39">
-        <v>0.51849608410944836</v>
+        <v>0.5184960841094484</v>
       </c>
       <c r="G39">
-        <v>0.49239042555107598</v>
+        <v>0.492390425551076</v>
       </c>
       <c r="H39">
-        <v>0.31533182174999352</v>
+        <v>0.3153318217499935</v>
       </c>
       <c r="I39">
-        <v>2.116575908640873E-2</v>
+        <v>0.02116575908640873</v>
       </c>
       <c r="J39">
-        <v>2.7038150759824891E-2</v>
+        <v>0.02703815075982489</v>
       </c>
       <c r="K39">
-        <v>3.001360983664618E-2</v>
+        <v>0.03001360983664618</v>
       </c>
       <c r="L39">
-        <v>2.8871542354218491E-2</v>
+        <v>0.02887154235421849</v>
       </c>
       <c r="M39">
-        <v>1.4762432562350981E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
+        <v>0.01476243256235098</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D40">
-        <v>8.2638752524127501E-2</v>
+        <v>0.0826387525241275</v>
       </c>
       <c r="E40">
-        <v>8.0133341235596539E-2</v>
+        <v>0.08013334123559654</v>
       </c>
       <c r="F40">
-        <v>6.9860168091991526E-2</v>
+        <v>0.06986016809199153</v>
       </c>
       <c r="G40">
-        <v>3.4711616893438553E-2</v>
+        <v>0.03471161689343855</v>
       </c>
       <c r="H40">
-        <v>2.3577554334068249E-2</v>
+        <v>0.02357755433406825</v>
       </c>
       <c r="I40">
-        <v>1.507743600230581E-2</v>
+        <v>0.01507743600230581</v>
       </c>
       <c r="J40">
-        <v>1.887656367852647E-2</v>
+        <v>0.01887656367852647</v>
       </c>
       <c r="K40">
-        <v>1.9620807475821341E-2</v>
+        <v>0.01962080747582134</v>
       </c>
       <c r="L40">
-        <v>1.6909744647706559E-2</v>
+        <v>0.01690974464770656</v>
       </c>
       <c r="M40">
-        <v>9.1554235029607071E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+        <v>0.009155423502960707</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
         <v>22</v>
       </c>
@@ -2001,33 +1974,33 @@
         <v>0.1182063477155845</v>
       </c>
       <c r="F41">
-        <v>9.5267378760850896E-2</v>
+        <v>0.0952673787608509</v>
       </c>
       <c r="G41">
-        <v>8.9617496288355497E-2</v>
+        <v>0.0896174962883555</v>
       </c>
       <c r="H41">
-        <v>8.0093840905438432E-2</v>
+        <v>0.08009384090543843</v>
       </c>
       <c r="I41">
-        <v>7.7951559659592107E-2</v>
+        <v>0.07795155965959211</v>
       </c>
       <c r="J41">
-        <v>6.6779495700166613E-2</v>
+        <v>0.06677949570016661</v>
       </c>
       <c r="K41">
-        <v>5.8654927263308863E-2</v>
+        <v>0.05865492726330886</v>
       </c>
       <c r="L41">
-        <v>5.4059061169731949E-2</v>
+        <v>0.05405906116973195</v>
       </c>
       <c r="M41">
-        <v>5.1111782642552922E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+        <v>0.05111178264255292</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
         <v>23</v>
       </c>
@@ -2035,297 +2008,297 @@
         <v>0.2162691048593598</v>
       </c>
       <c r="E42">
-        <v>0.19954699045935931</v>
+        <v>0.1995469904593593</v>
       </c>
       <c r="F42">
-        <v>0.20290676391408169</v>
+        <v>0.2029067639140817</v>
       </c>
       <c r="G42">
-        <v>0.18249700849866249</v>
+        <v>0.1824970084986625</v>
       </c>
       <c r="H42">
         <v>0.169289537802536</v>
       </c>
       <c r="I42">
-        <v>0.18573091070844769</v>
+        <v>0.1857309107084477</v>
       </c>
       <c r="J42">
-        <v>0.17630564183738839</v>
+        <v>0.1763056418373884</v>
       </c>
       <c r="K42">
-        <v>0.15888850717916911</v>
+        <v>0.1588885071791691</v>
       </c>
       <c r="L42">
         <v>0.144615300326741</v>
       </c>
       <c r="M42">
-        <v>0.13236342723550809</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+        <v>0.1323634272355081</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D43">
-        <v>2.6718865368589681E-2</v>
+        <v>0.02671886536858968</v>
       </c>
       <c r="E43">
-        <v>2.4307024033200241E-2</v>
+        <v>0.02430702403320024</v>
       </c>
       <c r="F43">
-        <v>1.5796700428466971E-2</v>
+        <v>0.01579670042846697</v>
       </c>
       <c r="G43">
-        <v>8.4348228141609485E-3</v>
+        <v>0.008434822814160949</v>
       </c>
       <c r="H43">
-        <v>7.7734230023658443E-3</v>
+        <v>0.007773423002365844</v>
       </c>
       <c r="I43">
-        <v>1.060333616994151E-2</v>
+        <v>0.01060333616994151</v>
       </c>
       <c r="J43">
-        <v>9.8291068853500058E-3</v>
+        <v>0.009829106885350006</v>
       </c>
       <c r="K43">
-        <v>6.3516311405392694E-3</v>
+        <v>0.006351631140539269</v>
       </c>
       <c r="L43">
-        <v>4.1837434586823301E-3</v>
+        <v>0.00418374345868233</v>
       </c>
       <c r="M43">
-        <v>2.78844444607585E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+        <v>0.00278844444607585</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="G44">
-        <v>5.3927056164761612E-3</v>
+        <v>0.005392705616476161</v>
       </c>
       <c r="H44">
-        <v>1.1327819003792219E-2</v>
+        <v>0.01132781900379222</v>
       </c>
       <c r="I44">
-        <v>1.821659055329572E-2</v>
+        <v>0.01821659055329572</v>
       </c>
       <c r="J44">
-        <v>1.9942130969237599E-2</v>
+        <v>0.0199421309692376</v>
       </c>
       <c r="K44">
-        <v>1.805379452882706E-2</v>
+        <v>0.01805379452882706</v>
       </c>
       <c r="L44">
-        <v>1.580334738808022E-2</v>
+        <v>0.01580334738808022</v>
       </c>
       <c r="M44">
-        <v>1.295709498676703E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+        <v>0.01295709498676703</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D45">
-        <v>2.2360774608925441E-6</v>
+        <v>2.236077460892544E-06</v>
       </c>
       <c r="E45">
-        <v>1.471425403057365E-3</v>
+        <v>0.001471425403057365</v>
       </c>
       <c r="F45">
-        <v>1.560166789281401E-2</v>
+        <v>0.01560166789281401</v>
       </c>
       <c r="G45">
-        <v>2.6981346757533171E-2</v>
+        <v>0.02698134675753317</v>
       </c>
       <c r="H45">
-        <v>0.14485733829161859</v>
+        <v>0.1448573382916186</v>
       </c>
       <c r="I45">
-        <v>0.32118813111604949</v>
+        <v>0.3211881311160495</v>
       </c>
       <c r="J45">
         <v>0.2936465128257244</v>
       </c>
       <c r="K45">
-        <v>0.29009404942272521</v>
+        <v>0.2900940494227252</v>
       </c>
       <c r="L45">
-        <v>0.29410894088426581</v>
+        <v>0.2941089408842658</v>
       </c>
       <c r="M45">
-        <v>0.31422335942713059</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
+        <v>0.3142233594271306</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D46">
-        <v>6.4846507240138261E-4</v>
+        <v>0.0006484650724013826</v>
       </c>
       <c r="E46">
-        <v>9.3248942612213087E-3</v>
+        <v>0.009324894261221309</v>
       </c>
       <c r="F46">
-        <v>5.2334353706493912E-2</v>
+        <v>0.05233435370649391</v>
       </c>
       <c r="G46">
-        <v>0.14728158496415211</v>
+        <v>0.1472815849641521</v>
       </c>
       <c r="H46">
-        <v>0.23272729606894571</v>
+        <v>0.2327272960689457</v>
       </c>
       <c r="I46">
-        <v>0.32119982596994889</v>
+        <v>0.3211998259699489</v>
       </c>
       <c r="J46">
-        <v>0.35977882449590809</v>
+        <v>0.3597788244959081</v>
       </c>
       <c r="K46">
-        <v>0.38620578319108162</v>
+        <v>0.3862057831910816</v>
       </c>
       <c r="L46">
-        <v>0.40613403776649781</v>
+        <v>0.4061340377664978</v>
       </c>
       <c r="M46">
         <v>0.4210589573583125</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2" t="s">
+    <row r="47" spans="1:13">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D47">
-        <v>1.785906178492112E-2</v>
+        <v>0.01785906178492112</v>
       </c>
       <c r="E47">
-        <v>2.8010555326487122E-2</v>
+        <v>0.02801055532648712</v>
       </c>
       <c r="F47">
-        <v>3.016754530783124E-2</v>
+        <v>0.03016754530783124</v>
       </c>
       <c r="G47">
-        <v>1.101068180667408E-2</v>
+        <v>0.01101068180667408</v>
       </c>
       <c r="H47">
-        <v>1.096514060516591E-2</v>
+        <v>0.01096514060516591</v>
       </c>
       <c r="I47">
-        <v>1.045188161491967E-2</v>
+        <v>0.01045188161491967</v>
       </c>
       <c r="J47">
-        <v>1.441027789350628E-2</v>
+        <v>0.01441027789350628</v>
       </c>
       <c r="K47">
-        <v>1.9517796337399591E-2</v>
+        <v>0.01951779633739959</v>
       </c>
       <c r="L47">
-        <v>2.2957828721051541E-2</v>
+        <v>0.02295782872105154</v>
       </c>
       <c r="M47">
-        <v>2.4249955006151201E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
+        <v>0.0242499550061512</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D48">
-        <v>0.25688365386153028</v>
+        <v>0.2568836538615303</v>
       </c>
       <c r="E48">
-        <v>0.20889703067180029</v>
+        <v>0.2088970306718003</v>
       </c>
       <c r="F48">
-        <v>0.22132362516024581</v>
+        <v>0.2213236251602458</v>
       </c>
       <c r="G48">
-        <v>0.16476936813768989</v>
+        <v>0.1647693681376899</v>
       </c>
       <c r="H48">
-        <v>9.2084769878816766E-2</v>
+        <v>0.09208476987881677</v>
       </c>
       <c r="I48">
-        <v>1.419594771127135E-3</v>
+        <v>0.001419594771127135</v>
       </c>
       <c r="J48">
-        <v>1.9838854824385721E-3</v>
+        <v>0.001983885482438572</v>
       </c>
       <c r="K48">
-        <v>2.1036505635947272E-3</v>
+        <v>0.002103650563594727</v>
       </c>
       <c r="L48">
-        <v>1.029273385830711E-3</v>
+        <v>0.001029273385830711</v>
       </c>
       <c r="M48">
-        <v>1.9453162904267839E-4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
+        <v>0.0001945316290426784</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D49">
-        <v>0.17687033328297669</v>
+        <v>0.1768703332829767</v>
       </c>
       <c r="E49">
         <v>0.2050483213169334</v>
       </c>
       <c r="F49">
-        <v>0.13971771430441729</v>
+        <v>0.1397177143044173</v>
       </c>
       <c r="G49">
-        <v>8.7708165104314881E-2</v>
+        <v>0.08770816510431488</v>
       </c>
       <c r="H49">
-        <v>2.9563834222922358E-2</v>
+        <v>0.02956383422292236</v>
       </c>
       <c r="I49">
-        <v>3.3163948286387048E-3</v>
+        <v>0.003316394828638705</v>
       </c>
       <c r="J49">
-        <v>2.924627440065801E-3</v>
+        <v>0.002924627440065801</v>
       </c>
       <c r="K49">
-        <v>2.250549540711974E-3</v>
+        <v>0.002250549540711974</v>
       </c>
       <c r="L49">
-        <v>1.37219841132239E-3</v>
+        <v>0.00137219841132239</v>
       </c>
       <c r="M49">
-        <v>5.2545422210795384E-4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
+        <v>0.0005254542221079538</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
         <v>22</v>
       </c>
@@ -2333,10 +2306,10 @@
         <v>0.1142238515239314</v>
       </c>
       <c r="E50">
-        <v>0.13748800473848591</v>
+        <v>0.1374880047384859</v>
       </c>
       <c r="F50">
-        <v>0.13045964957625031</v>
+        <v>0.1304596495762503</v>
       </c>
       <c r="G50">
         <v>0.1307371385261705</v>
@@ -2345,324 +2318,324 @@
         <v>0.1132273401965741</v>
       </c>
       <c r="I50">
-        <v>0.10058036721259821</v>
+        <v>0.1005803672125982</v>
       </c>
       <c r="J50">
-        <v>8.4533333760489007E-2</v>
+        <v>0.08453333376048901</v>
       </c>
       <c r="K50">
-        <v>7.1133896268123206E-2</v>
+        <v>0.07113389626812321</v>
       </c>
       <c r="L50">
-        <v>6.2312842544788222E-2</v>
+        <v>0.06231284254478822</v>
       </c>
       <c r="M50">
-        <v>5.5942604378623619E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
+        <v>0.05594260437862362</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D51">
-        <v>0.35909388046385382</v>
+        <v>0.3590938804638538</v>
       </c>
       <c r="E51">
-        <v>0.32805807533420822</v>
+        <v>0.3280580753342082</v>
       </c>
       <c r="F51">
-        <v>0.30887264850045698</v>
+        <v>0.308872648500457</v>
       </c>
       <c r="G51">
-        <v>0.29207893954587938</v>
+        <v>0.2920789395458794</v>
       </c>
       <c r="H51">
-        <v>0.26398153966667798</v>
+        <v>0.263981539666678</v>
       </c>
       <c r="I51">
-        <v>0.24008811116729151</v>
+        <v>0.2400881111672915</v>
       </c>
       <c r="J51">
-        <v>0.20897806082610271</v>
+        <v>0.2089780608261027</v>
       </c>
       <c r="K51">
-        <v>0.17596011721434551</v>
+        <v>0.1759601172143455</v>
       </c>
       <c r="L51">
-        <v>0.14918983736447369</v>
+        <v>0.1491898373644737</v>
       </c>
       <c r="M51">
         <v>0.1236718332359924</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D52">
-        <v>4.2588426355205149E-2</v>
+        <v>0.04258842635520515</v>
       </c>
       <c r="E52">
-        <v>2.247105381612529E-2</v>
+        <v>0.02247105381612529</v>
       </c>
       <c r="F52">
-        <v>1.9125103942189799E-2</v>
+        <v>0.0191251039421898</v>
       </c>
       <c r="G52">
-        <v>4.5556370259311994E-3</v>
+        <v>0.004555637025931199</v>
       </c>
       <c r="H52">
-        <v>2.096727292098235E-3</v>
+        <v>0.002096727292098235</v>
       </c>
       <c r="I52">
-        <v>1.472161626028177E-3</v>
+        <v>0.001472161626028177</v>
       </c>
       <c r="J52">
-        <v>1.8650979301141879E-3</v>
+        <v>0.001865097930114188</v>
       </c>
       <c r="K52">
-        <v>1.358090726857194E-3</v>
+        <v>0.001358090726857194</v>
       </c>
       <c r="L52">
-        <v>8.7699061829574643E-4</v>
+        <v>0.0008769906182957464</v>
       </c>
       <c r="M52">
-        <v>3.7001395636820369E-4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
+        <v>0.0003700139563682037</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D53">
-        <v>2.3652877936551171E-3</v>
+        <v>0.002365287793655117</v>
       </c>
       <c r="E53">
-        <v>2.406708427390982E-3</v>
+        <v>0.002406708427390982</v>
       </c>
       <c r="F53">
-        <v>2.934854985206594E-3</v>
+        <v>0.002934854985206594</v>
       </c>
       <c r="G53">
-        <v>1.1665697411576151E-2</v>
+        <v>0.01166569741157615</v>
       </c>
       <c r="H53">
-        <v>1.538310548301697E-2</v>
+        <v>0.01538310548301697</v>
       </c>
       <c r="I53">
-        <v>1.6228122006474031E-2</v>
+        <v>0.01622812200647403</v>
       </c>
       <c r="J53">
-        <v>1.7311989512766631E-2</v>
+        <v>0.01731198951276663</v>
       </c>
       <c r="K53">
-        <v>1.472526842842083E-2</v>
+        <v>0.01472526842842083</v>
       </c>
       <c r="L53">
-        <v>1.1507463043055629E-2</v>
+        <v>0.01150746304305563</v>
       </c>
       <c r="M53">
-        <v>7.8961539288934686E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
+        <v>0.007896153928893469</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D54">
-        <v>6.3898284017362649E-4</v>
+        <v>0.0006389828401736265</v>
       </c>
       <c r="E54">
-        <v>9.6904195248109504E-3</v>
+        <v>0.00969041952481095</v>
       </c>
       <c r="F54">
-        <v>4.1654964749589581E-2</v>
+        <v>0.04165496474958958</v>
       </c>
       <c r="G54">
-        <v>5.3235554429344772E-2</v>
+        <v>0.05323555442934477</v>
       </c>
       <c r="H54">
         <v>0.1491852344740297</v>
       </c>
       <c r="I54">
-        <v>0.23523523859681059</v>
+        <v>0.2352352385968106</v>
       </c>
       <c r="J54">
-        <v>0.23755568799786481</v>
+        <v>0.2375556879978648</v>
       </c>
       <c r="K54">
-        <v>0.25012007438790068</v>
+        <v>0.2501200743879007</v>
       </c>
       <c r="L54">
         <v>0.2814630265109288</v>
       </c>
       <c r="M54">
-        <v>0.34530828745720288</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
+        <v>0.3453082874572029</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D55">
-        <v>2.9476522093752872E-2</v>
+        <v>0.02947652209375287</v>
       </c>
       <c r="E55">
-        <v>5.7929830843757753E-2</v>
+        <v>0.05792983084375775</v>
       </c>
       <c r="F55">
         <v>0.1057438934738123</v>
       </c>
       <c r="G55">
-        <v>0.24423881801241909</v>
+        <v>0.2442388180124191</v>
       </c>
       <c r="H55">
-        <v>0.32351230818069793</v>
+        <v>0.3235123081806979</v>
       </c>
       <c r="I55">
-        <v>0.39120812817611211</v>
+        <v>0.3912081281761121</v>
       </c>
       <c r="J55">
         <v>0.4304370391566521</v>
       </c>
       <c r="K55">
-        <v>0.46283055653264638</v>
+        <v>0.4628305565326464</v>
       </c>
       <c r="L55">
-        <v>0.46929053940025328</v>
+        <v>0.4692905394002533</v>
       </c>
       <c r="M55">
-        <v>0.44184116618561758</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+        <v>0.4418411661856176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D56">
-        <v>6.111196806157358E-3</v>
+        <v>0.006111196806157358</v>
       </c>
       <c r="E56">
-        <v>2.0356177127053721E-2</v>
+        <v>0.02035617712705372</v>
       </c>
       <c r="F56">
-        <v>2.9736883095852599E-2</v>
+        <v>0.0297368830958526</v>
       </c>
       <c r="G56">
-        <v>1.269299261614506E-2</v>
+        <v>0.01269299261614506</v>
       </c>
       <c r="H56">
-        <v>1.502136884124145E-2</v>
+        <v>0.01502136884124145</v>
       </c>
       <c r="I56">
-        <v>2.9230819675679059E-2</v>
+        <v>0.02923081967567906</v>
       </c>
       <c r="J56">
-        <v>2.7696983199517529E-2</v>
+        <v>0.02769698319951753</v>
       </c>
       <c r="K56">
-        <v>3.2039564334934732E-2</v>
+        <v>0.03203956433493473</v>
       </c>
       <c r="L56">
-        <v>3.5223504469503841E-2</v>
+        <v>0.03522350446950384</v>
       </c>
       <c r="M56">
-        <v>4.1474039643214437E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
+        <v>0.04147403964321444</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D57">
-        <v>0.55969639602640198</v>
+        <v>0.559696396026402</v>
       </c>
       <c r="E57">
-        <v>0.54665379976492701</v>
+        <v>0.546653799764927</v>
       </c>
       <c r="F57">
-        <v>0.51849608410944836</v>
+        <v>0.5184960841094484</v>
       </c>
       <c r="G57">
-        <v>0.49239042555107598</v>
+        <v>0.492390425551076</v>
       </c>
       <c r="H57">
-        <v>0.31533182174999352</v>
+        <v>0.3153318217499935</v>
       </c>
       <c r="I57">
-        <v>2.0516107022041052E-2</v>
+        <v>0.02051610702204105</v>
       </c>
       <c r="J57">
-        <v>2.7226845021023349E-2</v>
+        <v>0.02722684502102335</v>
       </c>
       <c r="K57">
-        <v>3.0182405148858619E-2</v>
+        <v>0.03018240514885862</v>
       </c>
       <c r="L57">
-        <v>2.8901681629960121E-2</v>
+        <v>0.02890168162996012</v>
       </c>
       <c r="M57">
-        <v>1.4577714504510781E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
+        <v>0.01457771450451078</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D58">
-        <v>8.2638752524127501E-2</v>
+        <v>0.0826387525241275</v>
       </c>
       <c r="E58">
-        <v>8.0133341235596539E-2</v>
+        <v>0.08013334123559654</v>
       </c>
       <c r="F58">
-        <v>6.9860168091991526E-2</v>
+        <v>0.06986016809199153</v>
       </c>
       <c r="G58">
-        <v>3.4711616893438553E-2</v>
+        <v>0.03471161689343855</v>
       </c>
       <c r="H58">
-        <v>2.3577554334068249E-2</v>
+        <v>0.02357755433406825</v>
       </c>
       <c r="I58">
-        <v>1.501193167560041E-2</v>
+        <v>0.01501193167560041</v>
       </c>
       <c r="J58">
-        <v>1.919594927973936E-2</v>
+        <v>0.01919594927973936</v>
       </c>
       <c r="K58">
-        <v>1.9887363509893039E-2</v>
+        <v>0.01988736350989304</v>
       </c>
       <c r="L58">
-        <v>1.7046608823675799E-2</v>
+        <v>0.0170466088236758</v>
       </c>
       <c r="M58">
-        <v>9.1874723170729464E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
+        <v>0.009187472317072946</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
         <v>22</v>
       </c>
@@ -2673,33 +2646,33 @@
         <v>0.1182063477155845</v>
       </c>
       <c r="F59">
-        <v>9.5267378760850896E-2</v>
+        <v>0.0952673787608509</v>
       </c>
       <c r="G59">
-        <v>8.9617496288355497E-2</v>
+        <v>0.0896174962883555</v>
       </c>
       <c r="H59">
-        <v>8.0093840905438432E-2</v>
+        <v>0.08009384090543843</v>
       </c>
       <c r="I59">
-        <v>7.8002031858463911E-2</v>
+        <v>0.07800203185846391</v>
       </c>
       <c r="J59">
-        <v>6.6646257840123471E-2</v>
+        <v>0.06664625784012347</v>
       </c>
       <c r="K59">
-        <v>5.8436296623140732E-2</v>
+        <v>0.05843629662314073</v>
       </c>
       <c r="L59">
-        <v>5.3812486544440909E-2</v>
+        <v>0.05381248654444091</v>
       </c>
       <c r="M59">
-        <v>5.0834669235748767E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
+        <v>0.05083466923574877</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
         <v>23</v>
       </c>
@@ -2707,19 +2680,19 @@
         <v>0.2162691048593598</v>
       </c>
       <c r="E60">
-        <v>0.19954699045935931</v>
+        <v>0.1995469904593593</v>
       </c>
       <c r="F60">
-        <v>0.20290676391408169</v>
+        <v>0.2029067639140817</v>
       </c>
       <c r="G60">
-        <v>0.18249700849866249</v>
+        <v>0.1824970084986625</v>
       </c>
       <c r="H60">
         <v>0.169289537802536</v>
       </c>
       <c r="I60">
-        <v>0.18633316486337309</v>
+        <v>0.1863331648633731</v>
       </c>
       <c r="J60">
         <v>0.1765254195712013</v>
@@ -2728,276 +2701,276 @@
         <v>0.1590476653912766</v>
       </c>
       <c r="L60">
-        <v>0.14477849738622581</v>
+        <v>0.1447784973862258</v>
       </c>
       <c r="M60">
-        <v>0.13251494575687209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
+        <v>0.1325149457568721</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D61">
-        <v>2.6718865368589681E-2</v>
+        <v>0.02671886536858968</v>
       </c>
       <c r="E61">
-        <v>2.4307024033200241E-2</v>
+        <v>0.02430702403320024</v>
       </c>
       <c r="F61">
-        <v>1.5796700428466971E-2</v>
+        <v>0.01579670042846697</v>
       </c>
       <c r="G61">
-        <v>8.4348228141609485E-3</v>
+        <v>0.008434822814160949</v>
       </c>
       <c r="H61">
-        <v>7.7734230023658443E-3</v>
+        <v>0.007773423002365844</v>
       </c>
       <c r="I61">
-        <v>1.069492879764029E-2</v>
+        <v>0.01069492879764029</v>
       </c>
       <c r="J61">
-        <v>9.8593133197749979E-3</v>
+        <v>0.009859313319774998</v>
       </c>
       <c r="K61">
-        <v>6.4021801036759692E-3</v>
+        <v>0.006402180103675969</v>
       </c>
       <c r="L61">
-        <v>4.1994572485819486E-3</v>
+        <v>0.004199457248581949</v>
       </c>
       <c r="M61">
-        <v>2.796858501384216E-3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
+        <v>0.002796858501384216</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>1E-08</v>
       </c>
       <c r="G62">
-        <v>5.3927056164761612E-3</v>
+        <v>0.005392705616476161</v>
       </c>
       <c r="H62">
-        <v>1.1327819003792219E-2</v>
+        <v>0.01132781900379222</v>
       </c>
       <c r="I62">
-        <v>1.829999130028067E-2</v>
+        <v>0.01829999130028067</v>
       </c>
       <c r="J62">
-        <v>1.9941167736842891E-2</v>
+        <v>0.01994116773684289</v>
       </c>
       <c r="K62">
-        <v>1.8026038314611359E-2</v>
+        <v>0.01802603831461136</v>
       </c>
       <c r="L62">
-        <v>1.5764667080837728E-2</v>
+        <v>0.01576466708083773</v>
       </c>
       <c r="M62">
-        <v>1.2918840465667131E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
+        <v>0.01291884046566713</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D63">
-        <v>2.2360774608925441E-6</v>
+        <v>2.236077460892544E-06</v>
       </c>
       <c r="E63">
-        <v>1.471425403057365E-3</v>
+        <v>0.001471425403057365</v>
       </c>
       <c r="F63">
-        <v>1.560166789281401E-2</v>
+        <v>0.01560166789281401</v>
       </c>
       <c r="G63">
-        <v>2.6981346757533171E-2</v>
+        <v>0.02698134675753317</v>
       </c>
       <c r="H63">
-        <v>0.14485733829161859</v>
+        <v>0.1448573382916186</v>
       </c>
       <c r="I63">
-        <v>0.32065149670956611</v>
+        <v>0.3206514967095661</v>
       </c>
       <c r="J63">
         <v>0.2933644894213574</v>
       </c>
       <c r="K63">
-        <v>0.28979735470730722</v>
+        <v>0.2897973547073072</v>
       </c>
       <c r="L63">
-        <v>0.29397291003819409</v>
+        <v>0.2939729100381941</v>
       </c>
       <c r="M63">
-        <v>0.31428664257440542</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
+        <v>0.3142866425744054</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D64">
-        <v>6.4846507240138261E-4</v>
+        <v>0.0006484650724013826</v>
       </c>
       <c r="E64">
-        <v>9.3248942612213087E-3</v>
+        <v>0.009324894261221309</v>
       </c>
       <c r="F64">
-        <v>5.2334353706493912E-2</v>
+        <v>0.05233435370649391</v>
       </c>
       <c r="G64">
-        <v>0.14728158496415211</v>
+        <v>0.1472815849641521</v>
       </c>
       <c r="H64">
-        <v>0.23272729606894571</v>
+        <v>0.2327272960689457</v>
       </c>
       <c r="I64">
-        <v>0.32125952809735542</v>
+        <v>0.3212595280973554</v>
       </c>
       <c r="J64">
         <v>0.3595435746104198</v>
       </c>
       <c r="K64">
-        <v>0.38618113186630182</v>
+        <v>0.3861811318663018</v>
       </c>
       <c r="L64">
-        <v>0.40630018677857971</v>
+        <v>0.4063001867785797</v>
       </c>
       <c r="M64">
-        <v>0.42140881700112431</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2" t="s">
+        <v>0.4214088170011243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D65">
-        <v>1.785906178492112E-2</v>
+        <v>0.01785906178492112</v>
       </c>
       <c r="E65">
-        <v>2.8010555326487122E-2</v>
+        <v>0.02801055532648712</v>
       </c>
       <c r="F65">
-        <v>3.016754530783124E-2</v>
+        <v>0.03016754530783124</v>
       </c>
       <c r="G65">
-        <v>1.101068180667408E-2</v>
+        <v>0.01101068180667408</v>
       </c>
       <c r="H65">
-        <v>1.096514060516591E-2</v>
+        <v>0.01096514060516591</v>
       </c>
       <c r="I65">
-        <v>1.0622331714841921E-2</v>
+        <v>0.01062233171484192</v>
       </c>
       <c r="J65">
-        <v>1.4352759682747291E-2</v>
+        <v>0.01435275968274729</v>
       </c>
       <c r="K65">
-        <v>1.9465239654272229E-2</v>
+        <v>0.01946523965427223</v>
       </c>
       <c r="L65">
-        <v>2.2856261970142181E-2</v>
+        <v>0.02285626197014218</v>
       </c>
       <c r="M65">
-        <v>2.4102569075504791E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
+        <v>0.02410256907550479</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D66">
-        <v>0.25688365386153028</v>
+        <v>0.2568836538615303</v>
       </c>
       <c r="E66">
-        <v>0.20889703067180029</v>
+        <v>0.2088970306718003</v>
       </c>
       <c r="F66">
-        <v>0.22132362516024581</v>
+        <v>0.2213236251602458</v>
       </c>
       <c r="G66">
-        <v>0.16476936813768989</v>
+        <v>0.1647693681376899</v>
       </c>
       <c r="H66">
-        <v>9.2084769878816766E-2</v>
+        <v>0.09208476987881677</v>
       </c>
       <c r="I66">
-        <v>1.380347211112773E-3</v>
+        <v>0.001380347211112773</v>
       </c>
       <c r="J66">
-        <v>1.9887796901567412E-3</v>
+        <v>0.001988779690156741</v>
       </c>
       <c r="K66">
-        <v>2.1070327520948339E-3</v>
+        <v>0.002107032752094834</v>
       </c>
       <c r="L66">
-        <v>1.0140744616433041E-3</v>
+        <v>0.001014074461643304</v>
       </c>
       <c r="M66">
-        <v>1.9318080751149719E-4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
+        <v>0.0001931808075114972</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D67">
-        <v>0.17687033328297669</v>
+        <v>0.1768703332829767</v>
       </c>
       <c r="E67">
         <v>0.2050483213169334</v>
       </c>
       <c r="F67">
-        <v>0.13971771430441729</v>
+        <v>0.1397177143044173</v>
       </c>
       <c r="G67">
-        <v>8.7708165104314881E-2</v>
+        <v>0.08770816510431488</v>
       </c>
       <c r="H67">
-        <v>2.9563834222922358E-2</v>
+        <v>0.02956383422292236</v>
       </c>
       <c r="I67">
-        <v>3.1217406806747432E-3</v>
+        <v>0.003121740680674743</v>
       </c>
       <c r="J67">
-        <v>2.9801852296610148E-3</v>
+        <v>0.002980185229661015</v>
       </c>
       <c r="K67">
-        <v>2.2854630136471409E-3</v>
+        <v>0.002285463013647141</v>
       </c>
       <c r="L67">
-        <v>1.3792604795397399E-3</v>
+        <v>0.00137926047953974</v>
       </c>
       <c r="M67">
-        <v>5.2767554410324176E-4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
+        <v>0.0005276755441032418</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
         <v>22</v>
       </c>
@@ -3005,10 +2978,10 @@
         <v>0.1142238515239314</v>
       </c>
       <c r="E68">
-        <v>0.13748800473848591</v>
+        <v>0.1374880047384859</v>
       </c>
       <c r="F68">
-        <v>0.13045964957625031</v>
+        <v>0.1304596495762503</v>
       </c>
       <c r="G68">
         <v>0.1307371385261705</v>
@@ -3017,47 +2990,47 @@
         <v>0.1132273401965741</v>
       </c>
       <c r="I68">
-        <v>0.10053063943396159</v>
+        <v>0.1005306394339616</v>
       </c>
       <c r="J68">
-        <v>8.4326032907910548E-2</v>
+        <v>0.08432603290791055</v>
       </c>
       <c r="K68">
-        <v>7.0817530100720338E-2</v>
+        <v>0.07081753010072034</v>
       </c>
       <c r="L68">
-        <v>6.1913518712183903E-2</v>
+        <v>0.0619135187121839</v>
       </c>
       <c r="M68">
-        <v>5.5437154479615253E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
+        <v>0.05543715447961525</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D69">
-        <v>0.35909388046385382</v>
+        <v>0.3590938804638538</v>
       </c>
       <c r="E69">
-        <v>0.32805807533420822</v>
+        <v>0.3280580753342082</v>
       </c>
       <c r="F69">
-        <v>0.30887264850045698</v>
+        <v>0.308872648500457</v>
       </c>
       <c r="G69">
-        <v>0.29207893954587938</v>
+        <v>0.2920789395458794</v>
       </c>
       <c r="H69">
-        <v>0.26398153966667798</v>
+        <v>0.263981539666678</v>
       </c>
       <c r="I69">
-        <v>0.24026242173609741</v>
+        <v>0.2402624217360974</v>
       </c>
       <c r="J69">
-        <v>0.20892356211782481</v>
+        <v>0.2089235621178248</v>
       </c>
       <c r="K69">
         <v>0.175807570954784</v>
@@ -3069,152 +3042,152 @@
         <v>0.1232949078390875</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
+    <row r="70" spans="1:13">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D70">
-        <v>4.2588426355205149E-2</v>
+        <v>0.04258842635520515</v>
       </c>
       <c r="E70">
-        <v>2.247105381612529E-2</v>
+        <v>0.02247105381612529</v>
       </c>
       <c r="F70">
-        <v>1.9125103942189799E-2</v>
+        <v>0.0191251039421898</v>
       </c>
       <c r="G70">
-        <v>4.5556370259311994E-3</v>
+        <v>0.004555637025931199</v>
       </c>
       <c r="H70">
-        <v>2.096727292098235E-3</v>
+        <v>0.002096727292098235</v>
       </c>
       <c r="I70">
-        <v>1.481390816800881E-3</v>
+        <v>0.001481390816800881</v>
       </c>
       <c r="J70">
-        <v>1.87530171150343E-3</v>
+        <v>0.00187530171150343</v>
       </c>
       <c r="K70">
-        <v>1.36981067653322E-3</v>
+        <v>0.00136981067653322</v>
       </c>
       <c r="L70">
-        <v>8.8033148849629987E-4</v>
+        <v>0.0008803314884962999</v>
       </c>
       <c r="M70">
-        <v>3.7204532735269892E-4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
+        <v>0.0003720453273526989</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D71">
-        <v>2.3652877936551171E-3</v>
+        <v>0.002365287793655117</v>
       </c>
       <c r="E71">
-        <v>2.406708427390982E-3</v>
+        <v>0.002406708427390982</v>
       </c>
       <c r="F71">
-        <v>2.934854985206594E-3</v>
+        <v>0.002934854985206594</v>
       </c>
       <c r="G71">
-        <v>1.1665697411576151E-2</v>
+        <v>0.01166569741157615</v>
       </c>
       <c r="H71">
-        <v>1.538310548301697E-2</v>
+        <v>0.01538310548301697</v>
       </c>
       <c r="I71">
-        <v>1.629359005060366E-2</v>
+        <v>0.01629359005060366</v>
       </c>
       <c r="J71">
-        <v>1.7298104448794701E-2</v>
+        <v>0.0172981044487947</v>
       </c>
       <c r="K71">
-        <v>1.46943322479249E-2</v>
+        <v>0.0146943322479249</v>
       </c>
       <c r="L71">
-        <v>1.146478245380563E-2</v>
+        <v>0.01146478245380563</v>
       </c>
       <c r="M71">
-        <v>7.8546801393548672E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
+        <v>0.007854680139354867</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D72">
-        <v>6.3898284017362649E-4</v>
+        <v>0.0006389828401736265</v>
       </c>
       <c r="E72">
-        <v>9.6904195248109504E-3</v>
+        <v>0.00969041952481095</v>
       </c>
       <c r="F72">
-        <v>4.1654964749589581E-2</v>
+        <v>0.04165496474958958</v>
       </c>
       <c r="G72">
-        <v>5.3235554429344772E-2</v>
+        <v>0.05323555442934477</v>
       </c>
       <c r="H72">
         <v>0.1491852344740297</v>
       </c>
       <c r="I72">
-        <v>0.23526414086736019</v>
+        <v>0.2352641408673602</v>
       </c>
       <c r="J72">
-        <v>0.23783171381451829</v>
+        <v>0.2378317138145183</v>
       </c>
       <c r="K72">
         <v>0.2504263294798636</v>
       </c>
       <c r="L72">
-        <v>0.28203607830910671</v>
+        <v>0.2820360783091067</v>
       </c>
       <c r="M72">
-        <v>0.34627421065829472</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
+        <v>0.3462742106582947</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D73">
-        <v>2.9476522093752872E-2</v>
+        <v>0.02947652209375287</v>
       </c>
       <c r="E73">
-        <v>5.7929830843757753E-2</v>
+        <v>0.05792983084375775</v>
       </c>
       <c r="F73">
         <v>0.1057438934738123</v>
       </c>
       <c r="G73">
-        <v>0.24423881801241909</v>
+        <v>0.2442388180124191</v>
       </c>
       <c r="H73">
-        <v>0.32351230818069793</v>
+        <v>0.3235123081806979</v>
       </c>
       <c r="I73">
-        <v>0.39104339748854688</v>
+        <v>0.3910433974885469</v>
       </c>
       <c r="J73">
-        <v>0.43042356039688318</v>
+        <v>0.4304235603968832</v>
       </c>
       <c r="K73">
-        <v>0.46302669112015971</v>
+        <v>0.4630266911201597</v>
       </c>
       <c r="L73">
-        <v>0.46950777822047618</v>
+        <v>0.4695077782204762</v>
       </c>
       <c r="M73">
-        <v>0.44194357612917551</v>
+        <v>0.4419435761291755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>